<commit_message>
certificação da quantidade de dados
</commit_message>
<xml_diff>
--- a/Corona.xlsx
+++ b/Corona.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\Insper\2° semestre\CDados\Projetos\Projeto1_Cdados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{686A361D-AB75-459D-8C9C-3DD585EAA010}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF1625A3-9FD9-4F52-A509-F77220F8F2D7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Treinamento" sheetId="1" r:id="rId1"/>
@@ -4230,8 +4230,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D751"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="106" workbookViewId="0">
-      <selection activeCell="D678" sqref="D678"/>
+    <sheetView zoomScale="106" workbookViewId="0">
+      <selection activeCell="A750" sqref="A750"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10248,10 +10248,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D369"/>
+  <dimension ref="A1:D372"/>
   <sheetViews>
-    <sheetView topLeftCell="A364" zoomScale="117" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B369"/>
+    <sheetView tabSelected="1" topLeftCell="A348" zoomScale="117" workbookViewId="0">
+      <selection activeCell="A372" sqref="A372"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13210,6 +13210,18 @@
         <v>1116</v>
       </c>
     </row>
+    <row r="371" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A371" s="5">
+        <f>COUNTIF(A2:A369,1)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="372" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A372" s="5">
+        <f>COUNTIF(A2:A369,0)</f>
+        <v>267</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="C1:D1"/>

</xml_diff>